<commit_message>
Improved Reporting and Created second Test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EclipsePakage\eclipse-workspace\OrangeHRMTest\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650A541A-C3E5-499D-AB8D-D805134947D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE7697E-7869-4318-A99B-EDEE4793D76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Admin</t>
   </si>
@@ -34,12 +34,6 @@
   </si>
   <si>
     <t>pass</t>
-  </si>
-  <si>
-    <t>Admien</t>
-  </si>
-  <si>
-    <t>ademin123</t>
   </si>
   <si>
     <t>fail</t>
@@ -384,23 +378,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A4" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -416,35 +410,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
         <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>